<commit_message>
valid, invalid transactions displayed
</commit_message>
<xml_diff>
--- a/backend/clearingfeed (1).xlsx
+++ b/backend/clearingfeed (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\citibridge\citibridge\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8A83AB-AC3B-4596-83BF-F06FC3D825CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03844E59-E376-4D27-80BB-9F04AD7E7CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
   <si>
     <t>Anushka</t>
   </si>
@@ -93,9 +93,6 @@
     <t>123456743567</t>
   </si>
   <si>
-    <t>27/05/2023</t>
-  </si>
-  <si>
     <t>987654321989</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>875691.36</t>
   </si>
   <si>
-    <t>2023/05/29</t>
-  </si>
-  <si>
     <t>29/05/2023</t>
   </si>
   <si>
@@ -337,13 +331,16 @@
   </si>
   <si>
     <t>26484016912</t>
+  </si>
+  <si>
+    <t>2023/05/30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,7 +356,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -385,13 +396,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,419 +724,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7BB000-4A30-4982-86D3-BD9707B3B4E1}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="5" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="C14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="C16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>98</v>
-      </c>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
simple working home page
</commit_message>
<xml_diff>
--- a/backend/clearingfeed (1).xlsx
+++ b/backend/clearingfeed (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\citibridge\citibridge\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EEA001-8C52-4623-AB71-AC007FF79F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA0FD48-0AAC-4EAF-A62C-62AE510466E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
   </bookViews>
@@ -321,19 +321,19 @@
     <t>26484016912</t>
   </si>
   <si>
-    <t>31/05/2023</t>
-  </si>
-  <si>
-    <t>01/06/2023</t>
-  </si>
-  <si>
-    <t>2023/06/01</t>
-  </si>
-  <si>
-    <t>02/06/2023</t>
-  </si>
-  <si>
-    <t>06/01/2023</t>
+    <t>17/06/2023</t>
+  </si>
+  <si>
+    <t>2023/06/17</t>
+  </si>
+  <si>
+    <t>18/06/2023</t>
+  </si>
+  <si>
+    <t>06/17/2023</t>
+  </si>
+  <si>
+    <t>19/07/2023</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,7 +750,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>22</v>
@@ -775,7 +775,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>23</v>
@@ -800,7 +800,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>24</v>
@@ -825,7 +825,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>25</v>
@@ -850,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>26</v>
@@ -875,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>22</v>
@@ -899,8 +899,8 @@
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>99</v>
+      <c r="B7" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>37</v>
@@ -924,8 +924,8 @@
       <c r="A8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>99</v>
+      <c r="B8" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>50</v>
@@ -948,8 +948,8 @@
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>99</v>
+      <c r="B9" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>47</v>
@@ -972,8 +972,8 @@
       <c r="A10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>99</v>
+      <c r="B10" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>48</v>
@@ -996,8 +996,8 @@
       <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>99</v>
+      <c r="B11" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>49</v>
@@ -1021,7 +1021,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>58</v>
@@ -1045,7 +1045,7 @@
         <v>42</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>59</v>
@@ -1069,7 +1069,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>60</v>
@@ -1093,7 +1093,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>61</v>
@@ -1117,7 +1117,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>62</v>
@@ -1141,7 +1141,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Primary key of file table changed
</commit_message>
<xml_diff>
--- a/backend/clearingfeed (1).xlsx
+++ b/backend/clearingfeed (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\citibridge\citibridge\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA0FD48-0AAC-4EAF-A62C-62AE510466E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2407CA97-64F0-47FE-979A-F8F3A85FE734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
   </bookViews>
@@ -324,16 +324,16 @@
     <t>17/06/2023</t>
   </si>
   <si>
-    <t>2023/06/17</t>
-  </si>
-  <si>
     <t>18/06/2023</t>
   </si>
   <si>
-    <t>06/17/2023</t>
-  </si>
-  <si>
-    <t>19/07/2023</t>
+    <t>01/08/2023</t>
+  </si>
+  <si>
+    <t>2023/08/01</t>
+  </si>
+  <si>
+    <t>08/01/2023</t>
   </si>
 </sst>
 </file>
@@ -732,16 +732,17 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.453125" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -750,7 +751,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>22</v>
@@ -775,7 +776,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>23</v>
@@ -800,7 +801,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>24</v>
@@ -825,7 +826,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>25</v>
@@ -850,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>26</v>
@@ -875,7 +876,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>22</v>
@@ -900,7 +901,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>37</v>
@@ -925,7 +926,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>50</v>
@@ -973,7 +974,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>48</v>
@@ -997,7 +998,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>49</v>
@@ -1021,7 +1022,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>58</v>
@@ -1045,7 +1046,7 @@
         <v>42</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>59</v>
@@ -1069,7 +1070,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Horizontal navigation bar added
</commit_message>
<xml_diff>
--- a/backend/clearingfeed (1).xlsx
+++ b/backend/clearingfeed (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\citibridge\citibridge\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2407CA97-64F0-47FE-979A-F8F3A85FE734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB84B38-0743-4F09-AE6D-6C363D439B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
   </bookViews>
@@ -327,13 +327,13 @@
     <t>18/06/2023</t>
   </si>
   <si>
-    <t>01/08/2023</t>
-  </si>
-  <si>
-    <t>2023/08/01</t>
-  </si>
-  <si>
-    <t>08/01/2023</t>
+    <t>03/08/2023</t>
+  </si>
+  <si>
+    <t>2023/08/03</t>
+  </si>
+  <si>
+    <t>08/03/2023</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7BB000-4A30-4982-86D3-BD9707B3B4E1}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="122" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,7 +1117,7 @@
       <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1141,7 +1141,7 @@
       <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="8" t="s">

</xml_diff>

<commit_message>
UI changes, search bar and filters added
</commit_message>
<xml_diff>
--- a/backend/clearingfeed (1).xlsx
+++ b/backend/clearingfeed (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\citibridge\citibridge\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB84B38-0743-4F09-AE6D-6C363D439B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E748A15B-0179-45E2-9849-7E7EFD1DE02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74449CC9-AAE2-4CC1-9901-DAC8D6742FEE}"/>
   </bookViews>
@@ -327,13 +327,13 @@
     <t>18/06/2023</t>
   </si>
   <si>
-    <t>03/08/2023</t>
-  </si>
-  <si>
-    <t>2023/08/03</t>
-  </si>
-  <si>
-    <t>08/03/2023</t>
+    <t>06/08/2023</t>
+  </si>
+  <si>
+    <t>2023/08/06</t>
+  </si>
+  <si>
+    <t>08/06/2023</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="122" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B16" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>